<commit_message>
updated content and fixes
</commit_message>
<xml_diff>
--- a/src/data/careers.xlsx
+++ b/src/data/careers.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alroa\Desktop\WPRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FABD573E-5C07-4AAE-9E78-C88AE482F3F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AD923C6-1018-4D15-9AC6-8928C7595524}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="internships2019" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -56,9 +56,6 @@
     <t>Victor Shmulevich</t>
   </si>
   <si>
-    <t>Investment Banking Analyst</t>
-  </si>
-  <si>
     <t>Momentum Cyber</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>David Buzza</t>
   </si>
   <si>
-    <t>Joesph Cashore</t>
-  </si>
-  <si>
     <t>Tiffany Griesbach</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>Ayush Paliwal</t>
   </si>
   <si>
-    <t>Alexandria Li</t>
-  </si>
-  <si>
     <t>Jason Van</t>
   </si>
   <si>
@@ -107,9 +98,6 @@
     <t>Investment Banking Summer Analyst</t>
   </si>
   <si>
-    <t>Moelis</t>
-  </si>
-  <si>
     <t>Morgan Stanley</t>
   </si>
   <si>
@@ -146,9 +134,6 @@
     <t>Parm Sidhu</t>
   </si>
   <si>
-    <t>Padriac Lau</t>
-  </si>
-  <si>
     <t>Ali Cervienka</t>
   </si>
   <si>
@@ -161,9 +146,6 @@
     <t>Felicity Wang</t>
   </si>
   <si>
-    <t>Miguel Valaro</t>
-  </si>
-  <si>
     <t>Software Development Engineer Intern</t>
   </si>
   <si>
@@ -279,6 +261,24 @@
   </si>
   <si>
     <t>Kameel Ladak</t>
+  </si>
+  <si>
+    <t>HSBC</t>
+  </si>
+  <si>
+    <t>Joseph Cashore</t>
+  </si>
+  <si>
+    <t>Moelis &amp; Company</t>
+  </si>
+  <si>
+    <t>Alexandra Li</t>
+  </si>
+  <si>
+    <t>Padraic Lau</t>
+  </si>
+  <si>
+    <t>Miguel Valarao</t>
   </si>
 </sst>
 </file>
@@ -684,7 +684,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -719,466 +719,466 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" s="1"/>
     </row>

</xml_diff>